<commit_message>
add password protection and excel upload
</commit_message>
<xml_diff>
--- a/Content_Calendar.xlsx
+++ b/Content_Calendar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Desktop\content calendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48880507-3C8C-46D7-BEDA-948D19004381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958121C6-4A35-43DF-8172-92E721CD594B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38940" yWindow="3795" windowWidth="38700" windowHeight="15345" xr2:uid="{FA463503-EEA9-4E36-AF77-605EC82561F6}"/>
+    <workbookView xWindow="-38400" yWindow="3075" windowWidth="38700" windowHeight="15345" xr2:uid="{FA463503-EEA9-4E36-AF77-605EC82561F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Feed List" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="174">
   <si>
     <t>Category</t>
   </si>
@@ -519,9 +519,6 @@
   </si>
   <si>
     <t>"And hope does not disappoint us, because God has poured out his love into our hearts by the Holy Spirit, whom he has given us." \n\n- Romans 5:5 (NIV) #SundayScripture</t>
-  </si>
-  <si>
-    <t>Happy Friday! 💚</t>
   </si>
   <si>
     <t>“My children were malnourished and we hardly ate one meal a day,” says Betty in Uganda. \n\nBetty and Michal struggled to feed their daughters and pay school fees. But everything changed when kind people like you helped change their lives with gifts from the Food for the Hungry Gift Catalog.\n\nChickens to lay eggs. Seeds to grow vegetables. Tools and training to build a future.\n\n“Now we eat two meals a day. My children are healthy. We have hope,” Betty shares. 🫶 \n\nThis Christmas, you can give a gift that puts food on the table and changes lives.</t>
@@ -972,7 +969,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,9 +1111,7 @@
       <c r="F3" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>161</v>
-      </c>
+      <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
         <v>23</v>
       </c>
@@ -1166,7 +1161,7 @@
         <v>33</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>23</v>
@@ -1217,7 +1212,7 @@
         <v>37</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>23</v>
@@ -1268,7 +1263,7 @@
         <v>42</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>23</v>
@@ -1319,7 +1314,7 @@
         <v>45</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>23</v>
@@ -1370,7 +1365,7 @@
         <v>50</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>23</v>
@@ -1421,7 +1416,7 @@
         <v>54</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>23</v>
@@ -1472,7 +1467,7 @@
         <v>88</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>23</v>
@@ -1523,7 +1518,7 @@
         <v>61</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>23</v>
@@ -1574,7 +1569,7 @@
         <v>65</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>23</v>
@@ -1625,7 +1620,7 @@
         <v>69</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>23</v>
@@ -1676,7 +1671,7 @@
         <v>73</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>23</v>
@@ -1727,7 +1722,7 @@
         <v>77</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>23</v>
@@ -1778,7 +1773,7 @@
         <v>80</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
fix missing text links
</commit_message>
<xml_diff>
--- a/Content_Calendar.xlsx
+++ b/Content_Calendar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Desktop\content calendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CCD139-98FE-412A-A38D-7015430C64AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8679989-700A-402E-B4AA-6246D78F7734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39780" yWindow="3480" windowWidth="35550" windowHeight="15345" xr2:uid="{FA463503-EEA9-4E36-AF77-605EC82561F6}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="51840" windowHeight="21840" xr2:uid="{FA463503-EEA9-4E36-AF77-605EC82561F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Feed List" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="168">
   <si>
     <t>Category</t>
   </si>
@@ -393,9 +393,6 @@
   </si>
   <si>
     <t>When you give a Christmas gift 🎁 that makes room for love ❤️, you help lift families out of extreme poverty and bring real hope to entire communities.\n\nThe 2025 Gift Catalog is filled with meaningful ways to share the tangible love of Jesus with children and families facing overwhelming challenges.\n\nFrom goats that help families earn an income to chickens that provide daily nutrition, clean water that saves lives, school supplies that open doors to learning and Bibles that point families to lasting hope… every gift you choose can spark transformation that lasts for years.\n\nWill you make room this Christmas to help families take a giant step toward overcoming poverty and injustice?\n\nBrowse the Gift Catalog today and start giving gifts that change lives.</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
   <si>
     <t>Org_Giving_Dec10</t>
@@ -978,9 +975,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5370A7A5-E4F2-4D3A-BFE4-977B55C8323A}">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,7 +1111,7 @@
         <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>20</v>
@@ -1489,7 +1486,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1709,12 +1706,12 @@
       <c r="K15" s="2"/>
       <c r="L15" s="11"/>
       <c r="M15" s="2" t="s">
-        <v>118</v>
+        <v>23</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="O15" s="3" t="s">
         <v>58</v>
       </c>
       <c r="P15" s="3" t="s">
@@ -1878,7 +1875,7 @@
         <v>26</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>20</v>
@@ -1926,16 +1923,16 @@
         <v>26</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>22</v>
@@ -1983,7 +1980,7 @@
         <v>70</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>22</v>
@@ -2010,7 +2007,7 @@
         <v>23</v>
       </c>
       <c r="R21" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="135" x14ac:dyDescent="0.25">
@@ -2031,7 +2028,7 @@
         <v>72</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>22</v>
@@ -2046,10 +2043,10 @@
         <v>23</v>
       </c>
       <c r="N22" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="O22" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="O22" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="P22" s="3" t="s">
         <v>23</v>
@@ -2127,7 +2124,7 @@
         <v>31</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>22</v>
@@ -2145,7 +2142,7 @@
         <v>57</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P24" s="3" t="s">
         <v>23</v>
@@ -2271,7 +2268,7 @@
         <v>84</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>22</v>
@@ -2367,7 +2364,7 @@
         <v>43</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>22</v>
@@ -2415,7 +2412,7 @@
         <v>53</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>22</v>
@@ -2507,10 +2504,10 @@
         <v>20</v>
       </c>
       <c r="F32" t="s">
+        <v>133</v>
+      </c>
+      <c r="G32" t="s">
         <v>134</v>
-      </c>
-      <c r="G32" t="s">
-        <v>135</v>
       </c>
       <c r="H32" t="s">
         <v>22</v>
@@ -2534,7 +2531,7 @@
         <v>23</v>
       </c>
       <c r="R32" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -2545,16 +2542,16 @@
         <v>26</v>
       </c>
       <c r="D33" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" t="s">
         <v>137</v>
       </c>
-      <c r="E33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>138</v>
-      </c>
-      <c r="G33" t="s">
-        <v>139</v>
       </c>
       <c r="H33" t="s">
         <v>22</v>
@@ -2578,7 +2575,7 @@
         <v>23</v>
       </c>
       <c r="R33" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -2589,16 +2586,16 @@
         <v>26</v>
       </c>
       <c r="D34" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" t="s">
         <v>141</v>
       </c>
-      <c r="E34" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>142</v>
-      </c>
-      <c r="G34" t="s">
-        <v>143</v>
       </c>
       <c r="H34" t="s">
         <v>22</v>
@@ -2622,7 +2619,7 @@
         <v>23</v>
       </c>
       <c r="R34" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -2633,16 +2630,16 @@
         <v>26</v>
       </c>
       <c r="D35" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" t="s">
+        <v>163</v>
+      </c>
+      <c r="G35" t="s">
         <v>145</v>
-      </c>
-      <c r="E35" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" t="s">
-        <v>164</v>
-      </c>
-      <c r="G35" t="s">
-        <v>146</v>
       </c>
       <c r="H35" t="s">
         <v>22</v>
@@ -2666,7 +2663,7 @@
         <v>23</v>
       </c>
       <c r="R35" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
@@ -2677,16 +2674,16 @@
         <v>26</v>
       </c>
       <c r="D36" t="s">
+        <v>147</v>
+      </c>
+      <c r="E36" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" t="s">
         <v>148</v>
       </c>
-      <c r="E36" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>149</v>
-      </c>
-      <c r="G36" t="s">
-        <v>150</v>
       </c>
       <c r="H36" t="s">
         <v>22</v>
@@ -2710,7 +2707,7 @@
         <v>23</v>
       </c>
       <c r="R36" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -2721,16 +2718,16 @@
         <v>26</v>
       </c>
       <c r="D37" t="s">
+        <v>151</v>
+      </c>
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" t="s">
         <v>152</v>
       </c>
-      <c r="E37" t="s">
-        <v>20</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>153</v>
-      </c>
-      <c r="G37" t="s">
-        <v>154</v>
       </c>
       <c r="H37" t="s">
         <v>22</v>
@@ -2754,7 +2751,7 @@
         <v>23</v>
       </c>
       <c r="R37" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -2765,16 +2762,16 @@
         <v>26</v>
       </c>
       <c r="D38" t="s">
+        <v>155</v>
+      </c>
+      <c r="E38" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" t="s">
         <v>156</v>
       </c>
-      <c r="E38" t="s">
-        <v>20</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>157</v>
-      </c>
-      <c r="G38" t="s">
-        <v>158</v>
       </c>
       <c r="H38" t="s">
         <v>22</v>
@@ -2786,7 +2783,7 @@
         <v>22</v>
       </c>
       <c r="N38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O38" t="s">
         <v>58</v>
@@ -2809,16 +2806,16 @@
         <v>18</v>
       </c>
       <c r="D39" t="s">
+        <v>158</v>
+      </c>
+      <c r="E39" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" t="s">
         <v>159</v>
       </c>
-      <c r="E39" t="s">
-        <v>20</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>160</v>
-      </c>
-      <c r="G39" t="s">
-        <v>161</v>
       </c>
       <c r="H39" t="s">
         <v>22</v>
@@ -2842,7 +2839,7 @@
         <v>23</v>
       </c>
       <c r="R39" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -2853,16 +2850,16 @@
         <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E40" t="s">
         <v>20</v>
       </c>
       <c r="F40" t="s">
+        <v>166</v>
+      </c>
+      <c r="G40" t="s">
         <v>167</v>
-      </c>
-      <c r="G40" t="s">
-        <v>168</v>
       </c>
       <c r="H40" t="s">
         <v>22</v>
@@ -2887,7 +2884,7 @@
         <v>23</v>
       </c>
       <c r="R40" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2933,6 +2930,7 @@
     <hyperlink ref="R37" r:id="rId39" xr:uid="{AC7A4D61-C155-4165-8D8E-B7CFA56328D3}"/>
     <hyperlink ref="R38" r:id="rId40" xr:uid="{4759B8F6-371E-4EAA-B2F6-AECB0226A698}"/>
     <hyperlink ref="R39" r:id="rId41" xr:uid="{4B5AB1E8-8A1C-49D5-BC9B-CAC711736082}"/>
+    <hyperlink ref="O15" r:id="rId42" xr:uid="{B948F689-9ECB-4E36-809C-C2B9973B6F01}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>